<commit_message>
Update Activity diagrams, Log Bug and fix SearchFilter
</commit_message>
<xml_diff>
--- a/Documents/Testing Documents/Log Bug.xlsx
+++ b/Documents/Testing Documents/Log Bug.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="110" windowWidth="19140" windowHeight="7330"/>
+    <workbookView xWindow="0" yWindow="110" windowWidth="19140" windowHeight="7330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="5" r:id="rId1"/>
     <sheet name="06-05-2015" sheetId="1" r:id="rId2"/>
+    <sheet name="07-05-2015" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
   <si>
     <t>Bug Description</t>
   </si>
@@ -23,116 +24,128 @@
     <t>Files affected</t>
   </si>
   <si>
+    <t>Fixed By</t>
+  </si>
+  <si>
+    <t>LOG BUG</t>
+  </si>
+  <si>
+    <t>TEXAS GROUP</t>
+  </si>
+  <si>
+    <t>Last Update: 06/05/2015</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Additional Comment</t>
+  </si>
+  <si>
+    <t>Found Date</t>
+  </si>
+  <si>
+    <t>Fixed Date</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Complexity of Bug</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Created date: 06/05/2015</t>
+  </si>
+  <si>
+    <t>Complex</t>
+  </si>
+  <si>
+    <t>Very Complex</t>
+  </si>
+  <si>
+    <t>Can Duy Cat</t>
+  </si>
+  <si>
+    <t>Severity (1-5)</t>
+  </si>
+  <si>
+    <t>Controller 'ionNavBar', required by directive 'ionNavButtons', cant't be found.</t>
+  </si>
+  <si>
+    <t>Unexpected effects when load page</t>
+  </si>
+  <si>
+    <t>Unexpected effects when click on a card in FriendPanel</t>
+  </si>
+  <si>
+    <t>friend-panel.html</t>
+  </si>
+  <si>
+    <t>Month Calendar's day labels, Search Filter's avoid and prioritize buttons has wrong color when click on.</t>
+  </si>
+  <si>
+    <t>template-month.html, search-filter.html</t>
+  </si>
+  <si>
+    <t>search-filter.html,  my-profile.html.</t>
+  </si>
+  <si>
+    <t>Very Basic</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>Interface Bugs. Bugs can be fixed easily by CSS, HTML</t>
+  </si>
+  <si>
+    <t>Bugs affect some functions. Unable to run those functions. State that has these bugs may execute.</t>
+  </si>
+  <si>
+    <t>Bugs affect all functions of State. State that has these bugs cannot execute.Bugs are in library.</t>
+  </si>
+  <si>
+    <t>Bugs affect all functions of Application. Application cannot execute. Bugs have to be fixed immediately.</t>
+  </si>
+  <si>
+    <t>Data bugs. e.g., Missing files, images, cannot get or found data, etc.
+Logic bugs. Design bug.</t>
+  </si>
+  <si>
+    <t>Design bug: Message button's at Profile page of user. User sends message for themseft ?</t>
+  </si>
+  <si>
+    <t>Last Update: 07/05/2015</t>
+  </si>
+  <si>
+    <t>Nguyen Minh Trang</t>
+  </si>
+  <si>
     <t>Found By</t>
   </si>
   <si>
-    <t>Fixed By</t>
-  </si>
-  <si>
-    <t>LOG BUG</t>
-  </si>
-  <si>
-    <t>TEXAS GROUP</t>
-  </si>
-  <si>
-    <t>Last Update: 06/05/2015</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Severity</t>
-  </si>
-  <si>
-    <t>Additional Comment</t>
-  </si>
-  <si>
-    <t>Found Date</t>
-  </si>
-  <si>
-    <t>Fixed Date</t>
-  </si>
-  <si>
-    <t>Level</t>
-  </si>
-  <si>
-    <t>Normal</t>
-  </si>
-  <si>
-    <t>Complexity of Bug</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Created date: 06/05/2015</t>
-  </si>
-  <si>
-    <t>Bug affects all functions of Application. Application cannot execute. Bug have to be fixed immediately.</t>
-  </si>
-  <si>
-    <t>Bug affects some functions. Unable to run those functions. State that has this bug may execute.</t>
-  </si>
-  <si>
-    <t>Interface Bug. Bug can be fixed easily by CSS, HTML</t>
-  </si>
-  <si>
-    <t>Complex</t>
-  </si>
-  <si>
-    <t>Very Complex</t>
-  </si>
-  <si>
-    <t>Very Simple</t>
-  </si>
-  <si>
-    <t>Simple</t>
+    <t>Design bug: Do not reset data when click back function in event form</t>
   </si>
   <si>
     <t>Ngo Duc Dung</t>
   </si>
   <si>
-    <t>Can Duy Cat</t>
-  </si>
-  <si>
-    <t>Bug affects all functions of State. State that has this bug cannot execute.Bug is in library.</t>
-  </si>
-  <si>
-    <t>Severity (1-5)</t>
-  </si>
-  <si>
-    <t>Controller 'ionNavBar', required by directive 'ionNavButtons', cant't be found.</t>
-  </si>
-  <si>
-    <t>Unexpected effects when load page</t>
-  </si>
-  <si>
-    <t>todo.html</t>
-  </si>
-  <si>
-    <t>Unexpected effects when check on or click on star icons</t>
-  </si>
-  <si>
-    <t>Unexpected effects when click on a card in FriendPanel</t>
-  </si>
-  <si>
-    <t>friend-panel.html</t>
-  </si>
-  <si>
-    <t>Logic bug: Message button's at Profile page of user. User sends message for themseft ?</t>
-  </si>
-  <si>
-    <t>Month Calendar's day labels, Search Filter's avoid and prioritize buttons has wrong color when click on.</t>
-  </si>
-  <si>
-    <t>template-month.html, search-filter.html</t>
-  </si>
-  <si>
-    <t>Data bug. Eg: Missing files, images. Cannot get or found data…
-Logic bug.</t>
-  </si>
-  <si>
-    <t>search-filter.html,  my-profile.html.</t>
+    <t>search-filter.html, result.html</t>
+  </si>
+  <si>
+    <t>Design bug: Do not reset data when click back function in search-filter</t>
+  </si>
+  <si>
+    <t>Error when call getCalendar function: this.convertCal is not a function</t>
   </si>
 </sst>
 </file>
@@ -203,7 +216,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -242,21 +255,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -375,32 +373,6 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -483,66 +455,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -551,50 +621,98 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -899,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -913,11 +1031,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:10" ht="31" x14ac:dyDescent="0.7">
-      <c r="B3" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
+      <c r="B3" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -926,11 +1044,11 @@
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="2:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -939,11 +1057,11 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="2:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
+      <c r="B5" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -952,9 +1070,9 @@
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -963,37 +1081,37 @@
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="2:10" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
+      <c r="B7" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B8" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="21" t="s">
+      <c r="B8" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="23" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B9" s="20"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="24"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="32"/>
     </row>
     <row r="10" spans="2:10" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="6">
         <v>1</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="50" customHeight="1" x14ac:dyDescent="0.35">
@@ -1001,10 +1119,10 @@
         <v>2</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1012,10 +1130,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="35" customHeight="1" x14ac:dyDescent="0.35">
@@ -1023,10 +1141,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1034,10 +1152,10 @@
         <v>5</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1059,10 +1177,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J10"/>
+  <dimension ref="B2:J9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1073,129 +1191,107 @@
     <col min="4" max="4" width="43.6328125" customWidth="1"/>
     <col min="5" max="5" width="15.6328125" customWidth="1"/>
     <col min="6" max="6" width="26.26953125" customWidth="1"/>
-    <col min="7" max="9" width="17.453125" customWidth="1"/>
+    <col min="7" max="7" width="17.7265625" customWidth="1"/>
+    <col min="8" max="9" width="17.453125" customWidth="1"/>
     <col min="10" max="10" width="27.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="27" t="s">
+    <row r="2" spans="2:10" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+    </row>
+    <row r="3" spans="2:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-    </row>
-    <row r="2" spans="2:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="33" t="s">
+      <c r="C3" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="35" t="s">
+      <c r="J3" s="37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="28"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="38"/>
+    </row>
+    <row r="5" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="12">
         <v>1</v>
-      </c>
-      <c r="G2" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="20"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="30"/>
-    </row>
-    <row r="4" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="12">
-        <v>1</v>
-      </c>
-      <c r="C4" s="13">
-        <v>42130</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="11">
-        <v>1</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="17">
-        <v>42130</v>
-      </c>
-      <c r="J4" s="15"/>
-    </row>
-    <row r="5" spans="2:10" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="B5" s="12">
-        <v>2</v>
       </c>
       <c r="C5" s="13">
         <v>42130</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E5" s="11">
+        <v>1</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="16">
+        <v>42130</v>
+      </c>
+      <c r="J5" s="15"/>
+    </row>
+    <row r="6" spans="2:10" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B6" s="12">
         <v>2</v>
-      </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="15"/>
-    </row>
-    <row r="6" spans="2:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B6" s="12">
-        <v>3</v>
       </c>
       <c r="C6" s="13">
         <v>42130</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E6" s="11">
-        <v>1</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>24</v>
+        <v>2</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
@@ -1203,22 +1299,22 @@
     </row>
     <row r="7" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="13">
         <v>42130</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E7" s="11">
         <v>1</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
@@ -1232,65 +1328,224 @@
         <v>42130</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E8" s="11">
         <v>1</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="15"/>
     </row>
-    <row r="9" spans="2:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B9" s="12">
+    <row r="9" spans="2:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="57">
         <v>6</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="58">
         <v>42130</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="60">
         <v>2</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="15"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="12"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="15"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K7"/>
+  <sheetViews>
+    <sheetView zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="6.453125" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" customWidth="1"/>
+    <col min="4" max="4" width="43.6328125" customWidth="1"/>
+    <col min="5" max="5" width="15.6328125" customWidth="1"/>
+    <col min="6" max="6" width="26.26953125" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" customWidth="1"/>
+    <col min="8" max="9" width="17.453125" customWidth="1"/>
+    <col min="10" max="10" width="27.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" ht="29.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="23"/>
+    </row>
+    <row r="3" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="24"/>
+    </row>
+    <row r="4" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="48"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="55"/>
+    </row>
+    <row r="5" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="17">
+        <v>1</v>
+      </c>
+      <c r="C5" s="18">
+        <v>42131</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="19">
+        <v>2</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="21">
+        <v>42131</v>
+      </c>
+      <c r="J5" s="22"/>
+    </row>
+    <row r="6" spans="2:11" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="12">
+        <v>2</v>
+      </c>
+      <c r="C6" s="13">
+        <v>42131</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="11">
+        <v>3</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="16">
+        <v>42131</v>
+      </c>
+      <c r="J6" s="15"/>
+    </row>
+    <row r="7" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="57">
+        <v>3</v>
+      </c>
+      <c r="C7" s="58">
+        <v>42131</v>
+      </c>
+      <c r="D7" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="60">
+        <v>2</v>
+      </c>
+      <c r="F7" s="60"/>
+      <c r="G7" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="62">
+        <v>42131</v>
+      </c>
+      <c r="J7" s="63"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
update UML Activity + Log Bug, fix Search Filter and Friend panel
</commit_message>
<xml_diff>
--- a/Documents/Testing Documents/Log Bug.xlsx
+++ b/Documents/Testing Documents/Log Bug.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="110" windowWidth="19140" windowHeight="7330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="110" windowWidth="19140" windowHeight="7330" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="5" r:id="rId1"/>
     <sheet name="06-05-2015" sheetId="1" r:id="rId2"/>
     <sheet name="07-05-2015" sheetId="6" r:id="rId3"/>
+    <sheet name="09-05-2015" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
   <si>
     <t>Bug Description</t>
   </si>
@@ -146,6 +147,16 @@
   </si>
   <si>
     <t>Error when call getCalendar function: this.convertCal is not a function</t>
+  </si>
+  <si>
+    <t>edit-event.html, event-detail.html</t>
+  </si>
+  <si>
+    <t>When click edit button: "Cannot read property 'summary' of null".
+When click delete button: "Cannot read property 'events' of undefined".</t>
+  </si>
+  <si>
+    <t>Last Update: 09/05/2015</t>
   </si>
 </sst>
 </file>
@@ -529,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -597,6 +608,42 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -687,32 +734,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1031,11 +1057,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:10" ht="31" x14ac:dyDescent="0.7">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -1044,11 +1070,11 @@
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="2:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1057,11 +1083,11 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="2:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1070,9 +1096,9 @@
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1081,27 +1107,27 @@
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="2:10" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="43" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B9" s="28"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="32"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="44"/>
     </row>
     <row r="10" spans="2:10" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="6">
@@ -1179,8 +1205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1197,57 +1223,57 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
     </row>
     <row r="3" spans="2:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="39" t="s">
+      <c r="I3" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="37" t="s">
+      <c r="J3" s="49" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="28"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="50"/>
     </row>
     <row r="5" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B5" s="12">
@@ -1344,25 +1370,25 @@
       <c r="J8" s="15"/>
     </row>
     <row r="9" spans="2:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="57">
+      <c r="B9" s="25">
         <v>6</v>
       </c>
-      <c r="C9" s="58">
+      <c r="C9" s="26">
         <v>42130</v>
       </c>
-      <c r="D9" s="60" t="s">
+      <c r="D9" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="60">
+      <c r="E9" s="28">
         <v>2</v>
       </c>
-      <c r="F9" s="60"/>
-      <c r="G9" s="61" t="s">
+      <c r="F9" s="28"/>
+      <c r="G9" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="63"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1387,7 +1413,7 @@
   <dimension ref="B2:K7"/>
   <sheetViews>
     <sheetView zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1403,59 +1429,59 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="29.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
       <c r="K2" s="23"/>
     </row>
     <row r="3" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="51" t="s">
+      <c r="I3" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="56" t="s">
+      <c r="J3" s="67" t="s">
         <v>8</v>
       </c>
       <c r="K3" s="24"/>
     </row>
     <row r="4" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="48"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="55"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="68"/>
     </row>
     <row r="5" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="17">
@@ -1510,29 +1536,29 @@
       <c r="J6" s="15"/>
     </row>
     <row r="7" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="57">
+      <c r="B7" s="25">
         <v>3</v>
       </c>
-      <c r="C7" s="58">
+      <c r="C7" s="26">
         <v>42131</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="60">
+      <c r="E7" s="28">
         <v>2</v>
       </c>
-      <c r="F7" s="60"/>
-      <c r="G7" s="61" t="s">
+      <c r="F7" s="28"/>
+      <c r="G7" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="61" t="s">
+      <c r="H7" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="62">
+      <c r="I7" s="30">
         <v>42131</v>
       </c>
-      <c r="J7" s="63"/>
+      <c r="J7" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1550,4 +1576,118 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:J5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="6.453125" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" customWidth="1"/>
+    <col min="4" max="4" width="43.6328125" customWidth="1"/>
+    <col min="5" max="5" width="15.6328125" customWidth="1"/>
+    <col min="6" max="6" width="26.26953125" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" customWidth="1"/>
+    <col min="8" max="9" width="17.453125" customWidth="1"/>
+    <col min="10" max="10" width="27.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="65" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="67" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="60"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="68"/>
+    </row>
+    <row r="5" spans="2:10" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="32">
+        <v>1</v>
+      </c>
+      <c r="C5" s="33">
+        <v>42133</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="27">
+        <v>3</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="34"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="36"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>